<commit_message>
added the shape stencil size witth,height check to size the shape correctly. if you size the shape in Visio you should enter that Width,Height value into the shape Width, Height cells when the shape is drawn in the diagram the correct size will be used
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_ArchitectBlueprintingData_Templage2.xlsx
+++ b/Data/ScriptData/OC_ArchitectBlueprintingData_Templage2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0799438-903B-4EAD-9EDE-BA26AA6204D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C5648E-9C6E-43F3-AB94-EAC5927AC285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5010" yWindow="6390" windowWidth="23535" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4875" yWindow="2565" windowWidth="23535" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -2266,8 +2266,8 @@
   <dimension ref="A1:AJ57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2810,7 +2810,7 @@
         <v>9.4049999999999994</v>
       </c>
       <c r="U9" s="15">
-        <v>1.875</v>
+        <v>2.7</v>
       </c>
       <c r="V9" s="15">
         <v>6.5</v>

</xml_diff>

<commit_message>
added new stencil to the JSON file.   modified some PosX,PosY to the sample template
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_ArchitectBlueprintingData_Templage2.xlsx
+++ b/Data/ScriptData/OC_ArchitectBlueprintingData_Templage2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell_Blueprinting_Tool\Data\ScriptData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987A2BB5-F798-499F-9787-0C9664F4A40A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DD6010-A33A-4964-8875-9D6BC6BB12C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="6885" windowWidth="25665" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="6390" windowWidth="25665" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -230,7 +230,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="271">
   <si>
     <t>Shape</t>
   </si>
@@ -2270,8 +2270,8 @@
   <dimension ref="A1:AJ57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F36" sqref="F35:F36"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W51" sqref="W51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2870,7 +2870,7 @@
         <v>1.5</v>
       </c>
       <c r="U10" s="15">
-        <v>7</v>
+        <v>7.875</v>
       </c>
       <c r="V10" s="15">
         <v>0</v>
@@ -2979,11 +2979,19 @@
       </c>
       <c r="W12" s="13"/>
       <c r="X12" s="13"/>
-      <c r="Y12" s="13"/>
+      <c r="Y12" s="13" t="s">
+        <v>201</v>
+      </c>
       <c r="Z12" s="16"/>
-      <c r="AA12" s="16"/>
-      <c r="AB12" s="16"/>
-      <c r="AC12" s="16"/>
+      <c r="AA12" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB12" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC12" s="16" t="s">
+        <v>57</v>
+      </c>
       <c r="AD12" s="16"/>
       <c r="AE12" s="16"/>
       <c r="AF12" s="16"/>
@@ -3106,7 +3114,7 @@
         <v>104</v>
       </c>
       <c r="AB14" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AC14" s="11" t="s">
         <v>57</v>
@@ -3172,7 +3180,7 @@
         <v>104</v>
       </c>
       <c r="AB15" s="58" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AC15" s="58" t="s">
         <v>57</v>
@@ -3238,7 +3246,7 @@
         <v>104</v>
       </c>
       <c r="AB16" s="58" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AC16" s="58" t="s">
         <v>57</v>
@@ -4159,10 +4167,10 @@
         <v>5.875</v>
       </c>
       <c r="U30" s="27">
-        <v>0.125</v>
+        <v>0.5</v>
       </c>
       <c r="V30" s="27">
-        <v>0.125</v>
+        <v>0.6</v>
       </c>
       <c r="W30" s="11"/>
       <c r="X30" s="11"/>
@@ -5413,7 +5421,7 @@
         <v>66</v>
       </c>
       <c r="AI49" s="16" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="AJ49" s="16"/>
     </row>
@@ -5523,10 +5531,10 @@
       <c r="Q51" s="14"/>
       <c r="R51" s="16"/>
       <c r="S51" s="15">
-        <v>7.2709999999999999</v>
+        <v>6.75</v>
       </c>
       <c r="T51" s="15">
-        <v>8.5</v>
+        <v>8.4890000000000008</v>
       </c>
       <c r="U51" s="15">
         <v>0</v>

</xml_diff>